<commit_message>
Versión para vacaciones 2024
</commit_message>
<xml_diff>
--- a/AA - Calendario de Turnos(version Git_Hub 8).xlsx
+++ b/AA - Calendario de Turnos(version Git_Hub 8).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +482,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -517,13 +517,13 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Boettiger</t>
+          <t xml:space="preserve">  - Breinbauer</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -533,22 +533,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Feriado o Especial</t>
+          <t>Martes</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sin asignar</t>
+          <t>Iñiguez</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Sin asignar</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Feriado o Especial</t>
+          <t>Ramos</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -558,13 +558,13 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Boettiger</t>
+          <t xml:space="preserve">  - Breinbauer</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -574,22 +574,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Martes</t>
+          <t>Miércoles</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Arredondo</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -599,13 +599,13 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Boettiger</t>
+          <t xml:space="preserve">  - Iñiguez - Breinbauer - Carrasco</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -615,22 +615,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Miércoles</t>
+          <t>Jueves</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Fernandez</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Culaciati</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -640,13 +640,13 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger</t>
+          <t xml:space="preserve">  - Iñiguez - Breinbauer - Carrasco</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -656,22 +656,22 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Jueves</t>
+          <t>Viernes</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Carrasco</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -681,13 +681,13 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger</t>
+          <t xml:space="preserve">  - Iñiguez - Breinbauer - Carrasco</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -697,22 +697,22 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Viernes</t>
+          <t>Sábado</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -722,13 +722,13 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger</t>
+          <t xml:space="preserve">  - Iñiguez - Breinbauer - Carrasco</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -738,22 +738,22 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sábado</t>
+          <t>Domingo</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Fernandez</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Fernandez</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -763,13 +763,13 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger</t>
+          <t xml:space="preserve">  - Iñiguez - Breinbauer - Carrasco</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -779,7 +779,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Domingo</t>
+          <t>Lunes</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -789,12 +789,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Arredondo</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -804,13 +804,13 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Loch</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -820,22 +820,22 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Lunes</t>
+          <t>Martes</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Carrasco</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Culaciati</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -845,13 +845,13 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger - Loch</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Loch</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
@@ -861,24 +861,24 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Martes</t>
+          <t>Miércoles</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>Contreras</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Cisternas</t>
-        </is>
-      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t xml:space="preserve"> - </t>
@@ -886,13 +886,13 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger - Loch</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Loch</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -902,22 +902,22 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Miércoles</t>
+          <t>Jueves</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Fernandez</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Culaciati</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -927,13 +927,13 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger - Loch</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Loch</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -943,22 +943,22 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Jueves</t>
+          <t>Viernes</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Breinbauer</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -968,13 +968,13 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger - Loch</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Loch</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -984,22 +984,22 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Viernes</t>
+          <t>Sábado</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1009,13 +1009,13 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger - Loch</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Loch</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B15" t="n">
         <v>1</v>
@@ -1025,22 +1025,22 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Sábado</t>
+          <t>Domingo</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1050,13 +1050,13 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger - Loch - Rubio</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Ramos - Loch</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -1066,22 +1066,22 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Domingo</t>
+          <t>Lunes</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Gomez</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1091,13 +1091,13 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger - Loch - Rubio</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Cisternas - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
@@ -1107,22 +1107,22 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Lunes</t>
+          <t>Martes</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Carrasco</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1132,13 +1132,13 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Alvo - Ramos - Boettiger - Loch - Rubio</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Cisternas - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B18" t="n">
         <v>1</v>
@@ -1148,17 +1148,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Martes</t>
+          <t>Miércoles</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Arredondo</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1173,13 +1173,13 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Ramos - Boettiger - Loch - Rubio</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Cisternas - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B19" t="n">
         <v>1</v>
@@ -1189,22 +1189,22 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Miércoles</t>
+          <t>Jueves</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Fernandez</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Culaciati</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Carrasco</t>
+          <t>Culaciati</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1214,13 +1214,13 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Ramos - Boettiger - Loch - Rubio</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Cisternas - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B20" t="n">
         <v>1</v>
@@ -1230,22 +1230,22 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Jueves</t>
+          <t>Viernes</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Breinbauer</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1255,13 +1255,13 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Iñiguez - Boettiger - Loch - Rubio</t>
+          <t xml:space="preserve">  - Iñiguez - Carrasco - Cisternas - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B21" t="n">
         <v>1</v>
@@ -1271,22 +1271,22 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Viernes</t>
+          <t>Sábado</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1296,13 +1296,13 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Bravo - Iñiguez - Carrasco - Boettiger - Loch - Rubio</t>
+          <t xml:space="preserve">  - Gomez - Iñiguez - Carrasco - Cisternas - Pio - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B22" t="n">
         <v>1</v>
@@ -1312,22 +1312,22 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Sábado</t>
+          <t>Domingo</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1337,13 +1337,13 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Gomez - Bravo - Iñiguez - Carrasco - Boettiger - Loch - Rubio</t>
+          <t xml:space="preserve">  - Gomez - Iñiguez - Carrasco - Cisternas - Pio - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B23" t="n">
         <v>1</v>
@@ -1353,22 +1353,22 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Domingo</t>
+          <t>Lunes</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1378,13 +1378,13 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Gomez - Bravo - Iñiguez - Carrasco - Boettiger - Loch - Rubio</t>
+          <t xml:space="preserve">  - Gomez - Iñiguez - Carrasco - Cisternas - Pio - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B24" t="n">
         <v>1</v>
@@ -1394,22 +1394,22 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Lunes</t>
+          <t>Martes</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1419,13 +1419,13 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Gomez - Bravo - Iñiguez - Carrasco - Boettiger - Rubio</t>
+          <t xml:space="preserve">  - Gomez - Iñiguez - Carrasco - Cisternas - Pio - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B25" t="n">
         <v>1</v>
@@ -1435,22 +1435,22 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Martes</t>
+          <t>Miércoles</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Arredondo</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1460,13 +1460,13 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Gomez - Bravo - Iñiguez - Carrasco - Rubio</t>
+          <t xml:space="preserve">  - Gomez - Iñiguez - Carrasco - Cisternas - Pio - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B26" t="n">
         <v>1</v>
@@ -1476,22 +1476,22 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Miércoles</t>
+          <t>Jueves</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Fernandez</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Culaciati</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1501,13 +1501,13 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Gomez - Bravo - Iñiguez - Carrasco - Rubio</t>
+          <t xml:space="preserve">  - Gomez - Iñiguez - Carrasco - Cisternas - Pio - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B27" t="n">
         <v>1</v>
@@ -1517,22 +1517,22 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Jueves</t>
+          <t>Viernes</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Breinbauer</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Breinbauer</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1542,13 +1542,13 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Gomez - Bravo - Iñiguez - Carrasco - Rubio</t>
+          <t xml:space="preserve">  - Gomez - Iñiguez - Carrasco - Cisternas - Pio - Ramos - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B28" t="n">
         <v>1</v>
@@ -1558,24 +1558,24 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Viernes</t>
+          <t>Sábado</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>Bravo</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>Alvo</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Boettiger</t>
-        </is>
-      </c>
       <c r="H28" t="inlineStr">
         <is>
           <t xml:space="preserve"> - </t>
@@ -1583,13 +1583,13 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Gomez - Bravo - Iñiguez - Carrasco - Rubio</t>
+          <t xml:space="preserve">  - Gomez - Iñiguez - Carrasco - Cisternas - Pio - Ramos - Boettiger - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B29" t="n">
         <v>1</v>
@@ -1599,22 +1599,22 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Sábado</t>
+          <t>Domingo</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Breinbauer</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Breinbauer</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1624,13 +1624,13 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Gomez - Bravo - Iñiguez - Carrasco - Rubio</t>
+          <t xml:space="preserve">  - Gomez - Iñiguez - Carrasco - Cisternas - Pio - Ramos - Boettiger - Loch - Rubio</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B30" t="n">
         <v>1</v>
@@ -1640,22 +1640,22 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Domingo</t>
+          <t>Lunes</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Arredondo</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1665,13 +1665,13 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Gomez - Bravo - Iñiguez - Carrasco - Rubio</t>
+          <t xml:space="preserve">  - Gomez - Culaciati - Pio - Ramos - Boettiger - Loch</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B31" t="n">
         <v>1</v>
@@ -1681,22 +1681,22 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Lunes</t>
+          <t>Martes</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Iñiguez</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Contreras</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1706,13 +1706,13 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Iñiguez - Carrasco</t>
+          <t xml:space="preserve">  - Gomez - Culaciati - Pio - Ramos - Boettiger - Loch</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B32" t="n">
         <v>1</v>
@@ -1722,24 +1722,24 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Martes</t>
+          <t>Miércoles</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
           <t>Contreras</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Rubio</t>
-        </is>
-      </c>
       <c r="H32" t="inlineStr">
         <is>
           <t xml:space="preserve"> - </t>
@@ -1747,13 +1747,13 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Iñiguez - Carrasco</t>
+          <t xml:space="preserve">  - Gomez - Culaciati - Pio - Ramos - Boettiger - Loch</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B33" t="n">
         <v>2</v>
@@ -1763,22 +1763,22 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Miércoles</t>
+          <t>Jueves</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1788,13 +1788,13 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Carrasco - Culaciati - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger - Loch</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B34" t="n">
         <v>2</v>
@@ -1804,22 +1804,22 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Jueves</t>
+          <t>Viernes</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Breinbauer</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Arredondo</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1829,13 +1829,13 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Carrasco - Culaciati - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger - Loch</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B35" t="n">
         <v>2</v>
@@ -1845,22 +1845,22 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Viernes</t>
+          <t>Sábado</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1870,13 +1870,13 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Carrasco - Culaciati - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger - Loch</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B36" t="n">
         <v>2</v>
@@ -1886,22 +1886,22 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Sábado</t>
+          <t>Domingo</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1911,13 +1911,13 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Carrasco - Culaciati - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger - Loch</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B37" t="n">
         <v>2</v>
@@ -1927,22 +1927,22 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Domingo</t>
+          <t>Lunes</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1952,13 +1952,13 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Carrasco - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B38" t="n">
         <v>2</v>
@@ -1968,24 +1968,24 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Lunes</t>
+          <t>Martes</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
+          <t>Iñiguez</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Cisternas</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
           <t>Rubio</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Boettiger</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Ramos</t>
-        </is>
-      </c>
       <c r="H38" t="inlineStr">
         <is>
           <t xml:space="preserve"> - </t>
@@ -1993,13 +1993,13 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Carrasco - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B39" t="n">
         <v>2</v>
@@ -2009,22 +2009,22 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Martes</t>
+          <t>Miércoles</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2034,13 +2034,13 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Carrasco - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B40" t="n">
         <v>2</v>
@@ -2050,12 +2050,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Miércoles</t>
+          <t>Jueves</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2075,13 +2075,13 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Carrasco - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B41" t="n">
         <v>2</v>
@@ -2091,22 +2091,22 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Jueves</t>
+          <t>Viernes</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2116,13 +2116,13 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Carrasco - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B42" t="n">
         <v>2</v>
@@ -2132,22 +2132,22 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Viernes</t>
+          <t>Sábado</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2157,13 +2157,13 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Carrasco - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B43" t="n">
         <v>2</v>
@@ -2173,22 +2173,22 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Sábado</t>
+          <t>Domingo</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2198,13 +2198,13 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Carrasco - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B44" t="n">
         <v>2</v>
@@ -2214,22 +2214,22 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Domingo</t>
+          <t>Lunes</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2239,13 +2239,13 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Carrasco - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B45" t="n">
         <v>2</v>
@@ -2255,22 +2255,22 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Lunes</t>
+          <t>Martes</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
+          <t>Iñiguez</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
           <t>Rubio</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>Carrasco</t>
-        </is>
-      </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Boettiger</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2280,13 +2280,13 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B46" t="n">
         <v>2</v>
@@ -2296,22 +2296,22 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Martes</t>
+          <t>Miércoles</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Loch</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2321,13 +2321,13 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B47" t="n">
         <v>2</v>
@@ -2337,38 +2337,38 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Miércoles</t>
+          <t>Jueves</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - Pio con conflicto vacaciones -</t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Culaciati - Cisternas - Pio - Alvo</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B48" t="n">
         <v>2</v>
@@ -2378,22 +2378,22 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Jueves</t>
+          <t>Viernes</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
+          <t>Rubio</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
           <t>Alvo</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>Boettiger</t>
-        </is>
-      </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Alvo</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2403,13 +2403,13 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Culaciati - Cisternas - Pio</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B49" t="n">
         <v>2</v>
@@ -2419,12 +2419,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Viernes</t>
+          <t>Sábado</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2434,7 +2434,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Carrasco</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2444,13 +2444,13 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Bravo - Breinbauer - Arredondo - Culaciati - Cisternas - Pio</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B50" t="n">
         <v>2</v>
@@ -2460,22 +2460,22 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Sábado</t>
+          <t>Domingo</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2485,13 +2485,13 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Breinbauer - Arredondo - Culaciati - Cisternas - Pio</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B51" t="n">
         <v>2</v>
@@ -2501,22 +2501,22 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Domingo</t>
+          <t>Lunes</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
+          <t>Cisternas</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
           <t>Carrasco</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Carrasco</t>
-        </is>
-      </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Carrasco</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2526,13 +2526,13 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Gomez - Breinbauer - Arredondo - Culaciati - Cisternas - Pio</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Alvo - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B52" t="n">
         <v>2</v>
@@ -2542,22 +2542,22 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Lunes</t>
+          <t>Martes</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Iñiguez</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Carrasco</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -2567,13 +2567,13 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Breinbauer - Arredondo - Culaciati - Pio - Loch</t>
+          <t xml:space="preserve">  - Gomez - Breinbauer - Arredondo - Culaciati - Contreras - Alvo - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B53" t="n">
         <v>2</v>
@@ -2583,38 +2583,38 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Martes</t>
+          <t>Miércoles</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Contreras</t>
+          <t>Ramos</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones </t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Breinbauer - Arredondo - Culaciati - Pio - Loch</t>
+          <t xml:space="preserve">  - Breinbauer - Arredondo - Culaciati - Contreras - Alvo - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B54" t="n">
         <v>2</v>
@@ -2624,38 +2624,38 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Miércoles</t>
+          <t>Jueves</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Bravo</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - </t>
+          <t xml:space="preserve"> - Boettiger con conflicto vacaciones </t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Breinbauer - Arredondo - Culaciati - Pio - Loch</t>
+          <t xml:space="preserve">  - Breinbauer - Arredondo - Culaciati - Contreras - Alvo - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B55" t="n">
         <v>2</v>
@@ -2665,22 +2665,22 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Jueves</t>
+          <t>Viernes</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Cisternas</t>
+          <t>Loch</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Rubio</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2690,13 +2690,13 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Breinbauer - Arredondo - Culaciati - Pio - Loch</t>
+          <t xml:space="preserve">  - Breinbauer - Arredondo - Culaciati - Contreras - Alvo - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B56" t="n">
         <v>2</v>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Viernes</t>
+          <t>Sábado</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2716,28 +2716,28 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Rubio</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Bravo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - Pio con conflicto vacaciones -</t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Breinbauer - Arredondo - Culaciati - Pio - Loch</t>
+          <t xml:space="preserve">  - Breinbauer - Arredondo - Culaciati - Contreras - Alvo - Ramos - Boettiger</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B57" t="n">
         <v>2</v>
@@ -2747,22 +2747,22 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Sábado</t>
+          <t>Domingo</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Gomez</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Gomez</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2772,13 +2772,13 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Breinbauer - Arredondo - Culaciati - Pio - Loch</t>
+          <t xml:space="preserve">  - Breinbauer - Arredondo - Culaciati - Contreras - Alvo - Ramos</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B58" t="n">
         <v>2</v>
@@ -2788,38 +2788,38 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Domingo</t>
+          <t>Lunes</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Gomez</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Pio</t>
+          <t>Carrasco</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - Pio con conflicto vacaciones </t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Fernandez - Breinbauer - Arredondo - Culaciati - Pio - Loch</t>
+          <t xml:space="preserve">  - Arredondo - Culaciati - Contreras - Alvo - Ramos</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B59" t="n">
         <v>2</v>
@@ -2829,38 +2829,38 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Lunes</t>
+          <t>Martes</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Iñiguez</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Carrasco</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Breinbauer</t>
+          <t>Cisternas</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - Breinbauer con conflicto vacaciones </t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Loch</t>
+          <t xml:space="preserve">  - Arredondo - Contreras - Alvo - Ramos</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B60" t="n">
         <v>2</v>
@@ -2870,73 +2870,1385 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Martes</t>
+          <t>Miércoles</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Iñiguez</t>
+          <t>Fernandez</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Alvo</t>
+          <t>Boettiger</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Culaciati</t>
+          <t>Pio</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - Culaciati con conflicto vacaciones </t>
+          <t xml:space="preserve"> - </t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Breinbauer - Arredondo - Culaciati - Contreras - Pio - Loch</t>
+          <t xml:space="preserve">  - Arredondo - Contreras - Alvo - Ramos</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B61" t="n">
+        <v>2</v>
+      </c>
+      <c r="C61" t="n">
+        <v>29</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Jueves</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Bravo</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Loch</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Arredondo - Contreras - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B62" t="n">
         <v>3</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C62" t="n">
         <v>1</v>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Viernes</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Breinbauer</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Pio</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Rubio</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B63" t="n">
+        <v>3</v>
+      </c>
+      <c r="C63" t="n">
+        <v>2</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Sábado</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Iñiguez</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Iñiguez</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Cisternas</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B64" t="n">
+        <v>3</v>
+      </c>
+      <c r="C64" t="n">
+        <v>3</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Domingo</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3</v>
+      </c>
+      <c r="C65" t="n">
+        <v>4</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Lunes</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Gomez</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Carrasco</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Gomez</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B66" t="n">
+        <v>3</v>
+      </c>
+      <c r="C66" t="n">
+        <v>5</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Martes</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Iñiguez</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Contreras</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Iñiguez</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B67" t="n">
+        <v>3</v>
+      </c>
+      <c r="C67" t="n">
+        <v>6</v>
+      </c>
+      <c r="D67" t="inlineStr">
         <is>
           <t>Miércoles</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>Fernandez</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr">
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3</v>
+      </c>
+      <c r="C68" t="n">
+        <v>7</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Jueves</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
         <is>
           <t>Pio</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
         <is>
           <t>Pio</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - </t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  - Arredondo - Contreras - Loch</t>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B69" t="n">
+        <v>3</v>
+      </c>
+      <c r="C69" t="n">
+        <v>8</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Viernes</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Breinbauer</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B70" t="n">
+        <v>3</v>
+      </c>
+      <c r="C70" t="n">
+        <v>9</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Sábado</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B71" t="n">
+        <v>3</v>
+      </c>
+      <c r="C71" t="n">
+        <v>10</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Domingo</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Contreras</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Contreras</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Contreras</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B72" t="n">
+        <v>3</v>
+      </c>
+      <c r="C72" t="n">
+        <v>11</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Lunes</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Gomez</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Carrasco</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B73" t="n">
+        <v>3</v>
+      </c>
+      <c r="C73" t="n">
+        <v>12</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Martes</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Iñiguez</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Contreras</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B74" t="n">
+        <v>3</v>
+      </c>
+      <c r="C74" t="n">
+        <v>13</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Miércoles</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Fernandez</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Contreras</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B75" t="n">
+        <v>3</v>
+      </c>
+      <c r="C75" t="n">
+        <v>14</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Jueves</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Pio</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B76" t="n">
+        <v>3</v>
+      </c>
+      <c r="C76" t="n">
+        <v>15</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Viernes</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Breinbauer</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones </t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B77" t="n">
+        <v>3</v>
+      </c>
+      <c r="C77" t="n">
+        <v>16</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Sábado</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B78" t="n">
+        <v>3</v>
+      </c>
+      <c r="C78" t="n">
+        <v>17</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Domingo</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Loch</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Loch</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Loch</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Alvo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B79" t="n">
+        <v>3</v>
+      </c>
+      <c r="C79" t="n">
+        <v>18</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Lunes</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Gomez</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Carrasco</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B80" t="n">
+        <v>3</v>
+      </c>
+      <c r="C80" t="n">
+        <v>19</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Martes</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Iñiguez</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Contreras</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B81" t="n">
+        <v>3</v>
+      </c>
+      <c r="C81" t="n">
+        <v>20</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Miércoles</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Fernandez</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Contreras</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B82" t="n">
+        <v>3</v>
+      </c>
+      <c r="C82" t="n">
+        <v>21</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Jueves</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pio</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones -</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B83" t="n">
+        <v>3</v>
+      </c>
+      <c r="C83" t="n">
+        <v>22</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Viernes</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Breinbauer</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones </t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B84" t="n">
+        <v>3</v>
+      </c>
+      <c r="C84" t="n">
+        <v>23</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Sábado</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Pio</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Pio</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pio</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B85" t="n">
+        <v>3</v>
+      </c>
+      <c r="C85" t="n">
+        <v>24</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Domingo</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Boettiger</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B86" t="n">
+        <v>3</v>
+      </c>
+      <c r="C86" t="n">
+        <v>25</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Lunes</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Gomez</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Carrasco</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones </t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B87" t="n">
+        <v>3</v>
+      </c>
+      <c r="C87" t="n">
+        <v>26</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Martes</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Iñiguez</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Contreras</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones </t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B88" t="n">
+        <v>3</v>
+      </c>
+      <c r="C88" t="n">
+        <v>27</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Miércoles</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Fernandez</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Arredondo</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones </t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B89" t="n">
+        <v>3</v>
+      </c>
+      <c r="C89" t="n">
+        <v>28</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Jueves</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Culaciati</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones -Ramos con conflicto vacaciones </t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B90" t="n">
+        <v>3</v>
+      </c>
+      <c r="C90" t="n">
+        <v>29</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Feriado o Especial</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Sin asignar</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Sin asignar</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Feriado o Especial</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - </t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B91" t="n">
+        <v>3</v>
+      </c>
+      <c r="C91" t="n">
+        <v>30</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Sábado</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones </t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B92" t="n">
+        <v>3</v>
+      </c>
+      <c r="C92" t="n">
+        <v>31</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Domingo</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones </t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Bravo - Ramos</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B93" t="n">
+        <v>4</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Lunes</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Gomez</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Carrasco</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Ramos</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - Ramos con conflicto vacaciones </t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  - Ramos</t>
         </is>
       </c>
     </row>

</xml_diff>